<commit_message>
Modif ligne en trop horaire masso.xlsx
</commit_message>
<xml_diff>
--- a/excel/med_masso.xlsx
+++ b/excel/med_masso.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18006F10-903E-F748-ACC7-31329D63805C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F6B635-D4C0-6841-A77C-7F23D0A61561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39780" yWindow="2320" windowWidth="34040" windowHeight="24420" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
+    <workbookView xWindow="39780" yWindow="2320" windowWidth="34040" windowHeight="24420" activeTab="1" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
   <sheets>
     <sheet name="MEDICAL" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="16">
   <si>
     <t>code</t>
   </si>
@@ -168,9 +168,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -208,7 +208,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -314,7 +314,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -456,7 +456,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -466,7 +466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C23D3F-FE64-A34F-B126-68B68B58113C}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -585,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AEAFB22-B112-B74E-AFB9-7E6B7B7F9962}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -695,12 +695,6 @@
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>